<commit_message>
update services to create
</commit_message>
<xml_diff>
--- a/src/main/resources/guideline_base.xlsx
+++ b/src/main/resources/guideline_base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juan.estevez\Documents\IESS\OneDrive - Instituto Ecuatoriano de Seguridad Social\IESS\proyectos_git\guidelines\guidelines\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A223A499-4160-46C6-A0F0-51F2D2AE417C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4993B82-3817-404B-A3ED-4247589AD51A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">REVISADO POR: </t>
   </si>
   <si>
-    <t>Subdirector Nacional de Arquitectura y Soluciones</t>
-  </si>
-  <si>
     <t>Nombre - Cargo</t>
   </si>
   <si>
@@ -186,7 +183,10 @@
     <t>Juan Carlos Estevez</t>
   </si>
   <si>
-    <t>Wilson Xavier Villamil Quinteros</t>
+    <t>María Eufemia Ruales Proaño</t>
+  </si>
+  <si>
+    <t>Subdirectora Nacional de Arquitectura y Soluciones</t>
   </si>
 </sst>
 </file>
@@ -676,6 +676,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -699,30 +723,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1605,8 +1605,8 @@
   <dimension ref="A1:W44"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <pane ySplit="7" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -1628,81 +1628,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
-      <c r="C1" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="43" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="50" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="43"/>
+      <c r="H1" s="51"/>
     </row>
     <row r="2" spans="1:23" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="43"/>
+      <c r="H2" s="51"/>
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="1:23" s="1" customFormat="1" ht="9.4499999999999993" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
-      <c r="C3" s="44" t="s">
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="43" t="s">
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="43"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="4" spans="1:23" s="1" customFormat="1" ht="11.7" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="46"/>
-      <c r="G4" s="47" t="s">
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="48"/>
+      <c r="H4" s="56"/>
     </row>
     <row r="5" spans="1:23" ht="4.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
     </row>
     <row r="6" spans="1:23" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="54"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="56"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="46"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="48"/>
     </row>
     <row r="7" spans="1:23" s="6" customFormat="1" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -1718,7 +1718,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
@@ -1730,49 +1730,49 @@
         <v>13</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="2" t="s">
+      <c r="V7" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="W7" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:23" s="29" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.2">
@@ -2286,12 +2286,12 @@
     </row>
     <row r="29" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
+      <c r="F29" s="43"/>
       <c r="H29" s="9"/>
     </row>
     <row r="30" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2313,7 +2313,7 @@
     <row r="31" spans="1:23" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="C31" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>19</v>
@@ -2331,12 +2331,12 @@
       <c r="H32" s="9"/>
     </row>
     <row r="33" spans="3:8" ht="24.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="D33" s="50"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="51"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
+      <c r="F33" s="43"/>
       <c r="H33" s="9"/>
     </row>
     <row r="34" spans="3:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.2">
@@ -2356,7 +2356,7 @@
     </row>
     <row r="35" spans="3:8" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C35" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D35" s="16" t="s">
         <v>19</v>
@@ -2366,17 +2366,17 @@
       <c r="H35" s="9"/>
     </row>
     <row r="36" spans="3:8" ht="17.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51"/>
+      <c r="C36" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="43"/>
       <c r="H36" s="9"/>
     </row>
     <row r="37" spans="3:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C37" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D37" s="7" t="s">
         <v>16</v>
@@ -2391,10 +2391,10 @@
     </row>
     <row r="38" spans="3:8" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C38" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="18" t="s">
         <v>43</v>
-      </c>
-      <c r="D38" s="18" t="s">
-        <v>21</v>
       </c>
       <c r="E38" s="30"/>
       <c r="F38" s="19"/>
@@ -2423,12 +2423,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="A5:H5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:H6"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C33:F33"/>
     <mergeCell ref="A1:B4"/>
     <mergeCell ref="C1:F2"/>
     <mergeCell ref="G1:H1"/>
@@ -2437,6 +2431,12 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="A5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:H6"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="C33:F33"/>
   </mergeCells>
   <printOptions horizontalCentered="1" headings="1"/>
   <pageMargins left="0.17" right="0.16" top="5.185185185185185E-3" bottom="0.35" header="0.18" footer="0.5"/>

</xml_diff>